<commit_message>
updated cmax vs t experiment
</commit_message>
<xml_diff>
--- a/experiments/07_sched_method_comparison_4/Cmax_vs_T.xlsx
+++ b/experiments/07_sched_method_comparison_4/Cmax_vs_T.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_TEMP2\experiment_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3415DB1D-BF1B-4C0C-894F-95FCCC7AD181}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699E0763-9CA2-43A4-BA38-52FD2C53A678}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{0DDFCFBD-5BFA-484A-9640-7E9D9F2D067B}"/>
   </bookViews>
@@ -62,9 +62,6 @@
     <t>Major Frame length [ms]</t>
   </si>
   <si>
-    <t>C_max vs T_inf</t>
-  </si>
-  <si>
     <t>Resource Utilization</t>
   </si>
   <si>
@@ -84,6 +81,9 @@
   </si>
   <si>
     <t>Proc. time utilized</t>
+  </si>
+  <si>
+    <t>No B optimal + min Cmax</t>
   </si>
 </sst>
 </file>
@@ -1372,7 +1372,7 @@
         <c:axId val="349348240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="38"/>
+          <c:max val="39"/>
           <c:min val="25"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -3005,7 +3005,7 @@
   <dimension ref="A35:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3016,7 +3016,7 @@
   <sheetData>
     <row r="35" spans="1:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
@@ -3409,23 +3409,23 @@
     </row>
     <row r="45" spans="1:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C46" s="37"/>
       <c r="D46" s="40"/>
       <c r="E46" s="39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F46" s="37"/>
       <c r="G46" s="40"/>
       <c r="H46" s="39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I46" s="37"/>
       <c r="J46" s="38"/>
@@ -3435,31 +3435,31 @@
         <v>8</v>
       </c>
       <c r="B47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="D47" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D47" s="26" t="s">
-        <v>13</v>
-      </c>
       <c r="E47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="G47" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="G47" s="26" t="s">
-        <v>13</v>
-      </c>
       <c r="H47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I47" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I47" s="4" t="s">
+      <c r="J47" s="27" t="s">
         <v>12</v>
-      </c>
-      <c r="J47" s="27" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>